<commit_message>
update backlog + report
</commit_message>
<xml_diff>
--- a/Week 4/ProductBacklog (Version 0.5).xlsx
+++ b/Week 4/ProductBacklog (Version 0.5).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JavaWeb\swp391-onlineshop-gr1\Week 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT\SWP\swp391-onlineshop-gr1\Week 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B039F3-1C2F-4F3F-9CC9-E1AA597C019F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="76">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC (SWP391)</t>
   </si>
@@ -270,17 +271,27 @@
   <si>
     <t>02/010/2021</t>
   </si>
+  <si>
+    <t>Completed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="29" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -640,248 +651,248 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="12" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="13" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="28" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="28" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="28" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="29" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="29" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="29" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1237,11 +1248,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1904,7 +1915,7 @@
         <v>71</v>
       </c>
       <c r="H31" s="49" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="I31" s="74" t="s">
         <v>72</v>

</xml_diff>